<commit_message>
update import bantuan relawan
</commit_message>
<xml_diff>
--- a/excel/import_bantuan_relawan.xlsx
+++ b/excel/import_bantuan_relawan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Backend-PilkadaBanten\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FFD575-F462-42CC-9C74-2CE85AA533AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84975778-B43F-4583-91E5-60BEA8C728E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>tanggal</t>
   </si>
@@ -39,13 +39,19 @@
     <t>jenis_bantuan</t>
   </si>
   <si>
-    <t>jumlah</t>
-  </si>
-  <si>
     <t>sasaran</t>
   </si>
   <si>
     <t>Lebak</t>
+  </si>
+  <si>
+    <t>harga_satuan</t>
+  </si>
+  <si>
+    <t>jumlah_penerima</t>
+  </si>
+  <si>
+    <t>jumlah_bantuan</t>
   </si>
 </sst>
 </file>
@@ -99,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -111,6 +117,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -393,57 +402,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1"/>
-      <c r="F1"/>
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="G1"/>
       <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="4">
         <v>45570</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45000</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>